<commit_message>
Incluye clases de layouts
</commit_message>
<xml_diff>
--- a/SEGUIMIENTO MOVILES.xlsx
+++ b/SEGUIMIENTO MOVILES.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82514543-E9F6-4511-8BC4-AABECF5A5DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3135" windowWidth="20490" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEGUIMIENTO" sheetId="2" r:id="rId1"/>
@@ -504,7 +504,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>